<commit_message>
All good and clean now
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1896157_ed_ac_uk/Documents/Rafael/Python/grand_cattle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1896157\OneDrive - University of Edinburgh\Rafael\Python\grand_cattle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
-    <sheet name="Cattle" sheetId="3" r:id="rId2"/>
+    <sheet name="Scenario" sheetId="3" r:id="rId2"/>
     <sheet name="FeedLibrary" sheetId="1" r:id="rId3"/>
     <sheet name="Parameters List" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
@@ -1235,61 +1235,6 @@
   </cellStyles>
   <dxfs count="70">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
@@ -1585,6 +1530,61 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -1667,7 +1667,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="A1:Q3"/>
   <tableColumns count="17">
     <tableColumn id="1" name="ID"/>
@@ -1693,70 +1693,70 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A1:BF219"/>
   <sortState ref="A2:BF219">
     <sortCondition ref="A4:A5"/>
   </sortState>
   <tableColumns count="58">
-    <tableColumn id="1" name="ID" dataDxfId="61"/>
-    <tableColumn id="2" name="Feed" dataDxfId="60"/>
-    <tableColumn id="4" name="IFN" dataDxfId="59"/>
-    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="58"/>
-    <tableColumn id="7" name="Forage, %DM" dataDxfId="57"/>
-    <tableColumn id="8" name="DM, %AF" dataDxfId="56"/>
-    <tableColumn id="16" name="CP, %DM" dataDxfId="55"/>
-    <tableColumn id="31" name="SP, %CP" dataDxfId="54"/>
-    <tableColumn id="29" name="ADICP, %CP" dataDxfId="53"/>
-    <tableColumn id="24" name="Sugars, %DM" dataDxfId="52"/>
-    <tableColumn id="25" name="OA, %DM" dataDxfId="51"/>
-    <tableColumn id="23" name="Fat, %DM" dataDxfId="50"/>
-    <tableColumn id="9" name="Ash, %DM" dataDxfId="49"/>
-    <tableColumn id="10" name="Starch, %DM" dataDxfId="48"/>
-    <tableColumn id="12" name="NDF, %DM" dataDxfId="47"/>
-    <tableColumn id="13" name="Lignin, %DM" dataDxfId="46"/>
-    <tableColumn id="14" name="TDN, %DM" dataDxfId="45"/>
-    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="44"/>
-    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="43"/>
-    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="42"/>
-    <tableColumn id="21" name="RUP, %CP" dataDxfId="41"/>
-    <tableColumn id="22" name="kd PB, %/h" dataDxfId="40"/>
-    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="39"/>
-    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="38"/>
-    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="37"/>
-    <tableColumn id="28" name="PBID, %" dataDxfId="36"/>
-    <tableColumn id="6" name="CB1ID, %" dataDxfId="35"/>
-    <tableColumn id="3" name="CB2ID, %" dataDxfId="34"/>
-    <tableColumn id="20" name="pef, %NDF" dataDxfId="33"/>
-    <tableColumn id="11" name="ARG, %DM" dataDxfId="32"/>
-    <tableColumn id="32" name="HIS, %DM" dataDxfId="31"/>
-    <tableColumn id="33" name="ILE, %DM" dataDxfId="30"/>
-    <tableColumn id="34" name="LEU, %DM" dataDxfId="29"/>
-    <tableColumn id="35" name="LYS, %DM" dataDxfId="28"/>
-    <tableColumn id="36" name="MET, %DM" dataDxfId="27"/>
-    <tableColumn id="37" name="CYS, %DM" dataDxfId="26"/>
-    <tableColumn id="38" name="PHE, %DM" dataDxfId="25"/>
-    <tableColumn id="39" name="TYR, %DM" dataDxfId="24"/>
-    <tableColumn id="40" name="THR, %DM" dataDxfId="23"/>
-    <tableColumn id="41" name="TRP, %DM" dataDxfId="22"/>
-    <tableColumn id="42" name="VAL, %DM" dataDxfId="21"/>
-    <tableColumn id="43" name="Ca, % DM" dataDxfId="20"/>
-    <tableColumn id="44" name="P, % DM" dataDxfId="19"/>
-    <tableColumn id="45" name="Mg, % DM" dataDxfId="18"/>
-    <tableColumn id="46" name="Cl, % DM" dataDxfId="17"/>
-    <tableColumn id="47" name="K, % DM" dataDxfId="16"/>
-    <tableColumn id="48" name="Na, % DM" dataDxfId="15"/>
-    <tableColumn id="49" name="S, % DM" dataDxfId="14"/>
-    <tableColumn id="50" name="Co, mg/kg" dataDxfId="13"/>
-    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="12"/>
-    <tableColumn id="52" name="I, mg/kg" dataDxfId="11"/>
-    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="10"/>
-    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="9"/>
-    <tableColumn id="55" name="Se, mg/kg" dataDxfId="8"/>
-    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="7"/>
-    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="6"/>
-    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="5"/>
-    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="4"/>
+    <tableColumn id="1" name="ID" dataDxfId="57"/>
+    <tableColumn id="2" name="Feed" dataDxfId="56"/>
+    <tableColumn id="4" name="IFN" dataDxfId="55"/>
+    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="54"/>
+    <tableColumn id="7" name="Forage, %DM" dataDxfId="53"/>
+    <tableColumn id="8" name="DM, %AF" dataDxfId="52"/>
+    <tableColumn id="16" name="CP, %DM" dataDxfId="51"/>
+    <tableColumn id="31" name="SP, %CP" dataDxfId="50"/>
+    <tableColumn id="29" name="ADICP, %CP" dataDxfId="49"/>
+    <tableColumn id="24" name="Sugars, %DM" dataDxfId="48"/>
+    <tableColumn id="25" name="OA, %DM" dataDxfId="47"/>
+    <tableColumn id="23" name="Fat, %DM" dataDxfId="46"/>
+    <tableColumn id="9" name="Ash, %DM" dataDxfId="45"/>
+    <tableColumn id="10" name="Starch, %DM" dataDxfId="44"/>
+    <tableColumn id="12" name="NDF, %DM" dataDxfId="43"/>
+    <tableColumn id="13" name="Lignin, %DM" dataDxfId="42"/>
+    <tableColumn id="14" name="TDN, %DM" dataDxfId="41"/>
+    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="40"/>
+    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="39"/>
+    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="38"/>
+    <tableColumn id="21" name="RUP, %CP" dataDxfId="37"/>
+    <tableColumn id="22" name="kd PB, %/h" dataDxfId="36"/>
+    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="35"/>
+    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="34"/>
+    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="33"/>
+    <tableColumn id="28" name="PBID, %" dataDxfId="32"/>
+    <tableColumn id="6" name="CB1ID, %" dataDxfId="31"/>
+    <tableColumn id="3" name="CB2ID, %" dataDxfId="30"/>
+    <tableColumn id="20" name="pef, %NDF" dataDxfId="29"/>
+    <tableColumn id="11" name="ARG, %DM" dataDxfId="28"/>
+    <tableColumn id="32" name="HIS, %DM" dataDxfId="27"/>
+    <tableColumn id="33" name="ILE, %DM" dataDxfId="26"/>
+    <tableColumn id="34" name="LEU, %DM" dataDxfId="25"/>
+    <tableColumn id="35" name="LYS, %DM" dataDxfId="24"/>
+    <tableColumn id="36" name="MET, %DM" dataDxfId="23"/>
+    <tableColumn id="37" name="CYS, %DM" dataDxfId="22"/>
+    <tableColumn id="38" name="PHE, %DM" dataDxfId="21"/>
+    <tableColumn id="39" name="TYR, %DM" dataDxfId="20"/>
+    <tableColumn id="40" name="THR, %DM" dataDxfId="19"/>
+    <tableColumn id="41" name="TRP, %DM" dataDxfId="18"/>
+    <tableColumn id="42" name="VAL, %DM" dataDxfId="17"/>
+    <tableColumn id="43" name="Ca, % DM" dataDxfId="16"/>
+    <tableColumn id="44" name="P, % DM" dataDxfId="15"/>
+    <tableColumn id="45" name="Mg, % DM" dataDxfId="14"/>
+    <tableColumn id="46" name="Cl, % DM" dataDxfId="13"/>
+    <tableColumn id="47" name="K, % DM" dataDxfId="12"/>
+    <tableColumn id="48" name="Na, % DM" dataDxfId="11"/>
+    <tableColumn id="49" name="S, % DM" dataDxfId="10"/>
+    <tableColumn id="50" name="Co, mg/kg" dataDxfId="9"/>
+    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="8"/>
+    <tableColumn id="52" name="I, mg/kg" dataDxfId="7"/>
+    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="6"/>
+    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="5"/>
+    <tableColumn id="55" name="Se, mg/kg" dataDxfId="4"/>
+    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="3"/>
+    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="2"/>
+    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="1"/>
+    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2291,8 +2291,8 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2485,7 +2485,7 @@
   </sheetPr>
   <dimension ref="A1:BF219"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
@@ -40731,10 +40731,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:BF219">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="1" stopIfTrue="1">
       <formula>ROW(A2)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="2" stopIfTrue="1">
       <formula>COLUMN(A2)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41055,6 +41055,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43da31f6e8d8dfaec40561525ce78865">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b58fc7e6f492e58d10793199fba37542" ns3:_="" ns4:_="">
     <xsd:import namespace="871f9270-bc3b-4105-9923-e7982e1cb312"/>
@@ -41257,22 +41272,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE8DA1A1-DD54-4881-BC06-911C3C5870BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41289,29 +41314,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
forgot to update one file
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -974,9 +974,6 @@
     <t>Max</t>
   </si>
   <si>
-    <t>Special Cost</t>
-  </si>
-  <si>
     <t>Breed</t>
   </si>
   <si>
@@ -1035,6 +1032,9 @@
   </si>
   <si>
     <t>LCA</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -1657,7 +1657,7 @@
     <tableColumn id="1" name="ID" dataDxfId="68"/>
     <tableColumn id="2" name="Min" dataDxfId="67"/>
     <tableColumn id="3" name="Max" dataDxfId="66"/>
-    <tableColumn id="4" name="Special Cost" dataDxfId="65"/>
+    <tableColumn id="4" name="Cost" dataDxfId="65"/>
     <tableColumn id="5" name="Name" dataDxfId="64">
       <calculatedColumnFormula>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
@@ -2030,20 +2030,20 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="H7:J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -2054,13 +2054,13 @@
         <v>314</v>
       </c>
       <c r="D1" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="E1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>34</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>Citrus pulp, dry</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>45</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>Corn grain</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>50</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>Corn silage</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>58</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>Cottonseed meal</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>59</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>Cottonseed whole</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>60</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>Distillers grain plus soluble, dry</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>79</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>Grain sorghum grain</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>133</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>Soybean hulls</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>134</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>Soybean meal high CP</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>148</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>Sugarcane silage</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>166</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>Wheat middlings</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>845</v>
       </c>
@@ -2291,85 +2291,85 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q13" sqref="O13:Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>318</v>
-      </c>
       <c r="E1" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="F1" s="26" t="s">
         <v>320</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>322</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="I1" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="J1" s="26" t="s">
         <v>324</v>
       </c>
-      <c r="J1" s="26" t="s">
-        <v>325</v>
-      </c>
       <c r="K1" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>327</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q1" s="31" t="s">
         <v>334</v>
       </c>
-      <c r="L1" s="28" t="s">
-        <v>328</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>327</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>331</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>332</v>
-      </c>
-      <c r="P1" s="28" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>335</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="24">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C2" s="24">
         <v>300</v>
@@ -2399,10 +2399,10 @@
         <v>13.91</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N2" s="23">
         <v>0.8</v>
@@ -2417,12 +2417,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C3" s="29">
         <v>300</v>
@@ -2452,10 +2452,10 @@
         <v>13.91</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N3" s="29">
         <v>0.8</v>
@@ -2489,63 +2489,63 @@
       <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="12" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="49" max="50" width="12" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="56" max="57" width="12" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>44.9</v>
       </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4983,7 +4983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -6201,7 +6201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -6723,7 +6723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -6897,7 +6897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -7245,7 +7245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -7593,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -7767,7 +7767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -7941,7 +7941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -8463,7 +8463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -8637,7 +8637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -8811,7 +8811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -8985,7 +8985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -9159,7 +9159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -9333,7 +9333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -9507,7 +9507,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -9681,7 +9681,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="42" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -9855,7 +9855,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -10029,7 +10029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -10203,7 +10203,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -10377,7 +10377,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -10551,7 +10551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -10725,7 +10725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -10899,7 +10899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -11073,7 +11073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -11421,7 +11421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -11595,7 +11595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -11769,7 +11769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -11943,7 +11943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -12117,7 +12117,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -12291,7 +12291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -12465,7 +12465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -12639,7 +12639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -12813,7 +12813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -12987,7 +12987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -13161,7 +13161,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="62" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -13335,7 +13335,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="63" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -13509,7 +13509,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="64" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -13683,7 +13683,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="65" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -13857,7 +13857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -14031,7 +14031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -14205,7 +14205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -14379,7 +14379,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -14553,7 +14553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -14727,7 +14727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -14901,7 +14901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -15075,7 +15075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -15249,7 +15249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -15423,7 +15423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -15597,7 +15597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -15771,7 +15771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -15945,7 +15945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -16119,7 +16119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -16293,7 +16293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -16467,7 +16467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -16641,7 +16641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -16815,7 +16815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -16989,7 +16989,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -17163,7 +17163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -17337,7 +17337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -17511,7 +17511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -17685,7 +17685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -17859,7 +17859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -18033,7 +18033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -18207,7 +18207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -18381,7 +18381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -18555,7 +18555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -18729,7 +18729,7 @@
         <v>135.6</v>
       </c>
     </row>
-    <row r="94" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -18903,7 +18903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -19077,7 +19077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -19251,7 +19251,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="97" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -19425,7 +19425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -19599,7 +19599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -19773,7 +19773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -19947,7 +19947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -20121,7 +20121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -20295,7 +20295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -20469,7 +20469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -20643,7 +20643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -20817,7 +20817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -20991,7 +20991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -21165,7 +21165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -21339,7 +21339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -21513,7 +21513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -21687,7 +21687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -21861,7 +21861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -22035,7 +22035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -22209,7 +22209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -22383,7 +22383,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -22557,7 +22557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -22731,7 +22731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -22905,7 +22905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -23079,7 +23079,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -23253,7 +23253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -23427,7 +23427,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="121" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -23601,7 +23601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -23775,7 +23775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -23949,7 +23949,7 @@
         <v>66.7</v>
       </c>
     </row>
-    <row r="124" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -24123,7 +24123,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="125" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -24297,7 +24297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -24471,7 +24471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -24645,7 +24645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -24819,7 +24819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -24993,7 +24993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -25167,7 +25167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -25341,7 +25341,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -25515,7 +25515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -25689,7 +25689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -25863,7 +25863,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="135" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -26037,7 +26037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -26211,7 +26211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -26385,7 +26385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -26559,7 +26559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -26733,7 +26733,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="140" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -26907,7 +26907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -27081,7 +27081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -27255,7 +27255,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="143" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -27429,7 +27429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -27603,7 +27603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -27777,7 +27777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -27951,7 +27951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -28125,7 +28125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -28299,7 +28299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -28473,7 +28473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -28647,7 +28647,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="151" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -28821,7 +28821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -28995,7 +28995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -29169,7 +29169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -29343,7 +29343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -29517,7 +29517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -29691,7 +29691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>156</v>
       </c>
@@ -29865,7 +29865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -30039,7 +30039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>158</v>
       </c>
@@ -30213,7 +30213,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="160" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>159</v>
       </c>
@@ -30387,7 +30387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>160</v>
       </c>
@@ -30561,7 +30561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>161</v>
       </c>
@@ -30735,7 +30735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>162</v>
       </c>
@@ -30909,7 +30909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>163</v>
       </c>
@@ -31083,7 +31083,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="165" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>164</v>
       </c>
@@ -31257,7 +31257,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="166" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>165</v>
       </c>
@@ -31431,7 +31431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>166</v>
       </c>
@@ -31605,7 +31605,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="168" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>167</v>
       </c>
@@ -31779,7 +31779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>168</v>
       </c>
@@ -31953,7 +31953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>169</v>
       </c>
@@ -32127,7 +32127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>170</v>
       </c>
@@ -32301,7 +32301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>800</v>
       </c>
@@ -32477,7 +32477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>801</v>
       </c>
@@ -32653,7 +32653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>802</v>
       </c>
@@ -32829,7 +32829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>803</v>
       </c>
@@ -33005,7 +33005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>804</v>
       </c>
@@ -33181,7 +33181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>805</v>
       </c>
@@ -33355,7 +33355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>806</v>
       </c>
@@ -33529,7 +33529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>807</v>
       </c>
@@ -33703,7 +33703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>808</v>
       </c>
@@ -33877,7 +33877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>809</v>
       </c>
@@ -34053,7 +34053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>810</v>
       </c>
@@ -34229,7 +34229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>811</v>
       </c>
@@ -34405,7 +34405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>812</v>
       </c>
@@ -34581,7 +34581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>813</v>
       </c>
@@ -34757,7 +34757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>814</v>
       </c>
@@ -34933,7 +34933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>815</v>
       </c>
@@ -35109,7 +35109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>816</v>
       </c>
@@ -35285,7 +35285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>817</v>
       </c>
@@ -35461,7 +35461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>818</v>
       </c>
@@ -35637,7 +35637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>819</v>
       </c>
@@ -35811,7 +35811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>820</v>
       </c>
@@ -35985,7 +35985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>821</v>
       </c>
@@ -36161,7 +36161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>822</v>
       </c>
@@ -36337,7 +36337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>823</v>
       </c>
@@ -36513,7 +36513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>824</v>
       </c>
@@ -36689,7 +36689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>825</v>
       </c>
@@ -36863,7 +36863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>826</v>
       </c>
@@ -37037,7 +37037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>827</v>
       </c>
@@ -37213,7 +37213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>828</v>
       </c>
@@ -37389,7 +37389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>829</v>
       </c>
@@ -37565,7 +37565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>830</v>
       </c>
@@ -37741,7 +37741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>831</v>
       </c>
@@ -37917,7 +37917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>832</v>
       </c>
@@ -38093,7 +38093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>833</v>
       </c>
@@ -38269,7 +38269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>834</v>
       </c>
@@ -38445,7 +38445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>835</v>
       </c>
@@ -38619,7 +38619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>836</v>
       </c>
@@ -38795,7 +38795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>837</v>
       </c>
@@ -38971,7 +38971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>838</v>
       </c>
@@ -39147,7 +39147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>839</v>
       </c>
@@ -39323,7 +39323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>840</v>
       </c>
@@ -39499,7 +39499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>841</v>
       </c>
@@ -39675,7 +39675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>842</v>
       </c>
@@ -39851,7 +39851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>843</v>
       </c>
@@ -40027,7 +40027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>844</v>
       </c>
@@ -40203,7 +40203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>845</v>
       </c>
@@ -40377,7 +40377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>846</v>
       </c>
@@ -40553,7 +40553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>847</v>
       </c>
@@ -40754,297 +40754,297 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>55</v>
       </c>
@@ -41055,12 +41055,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -41267,15 +41264,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -41300,18 +41309,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
-    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
linear_factor adjusted in nrc_equations.py and lb and ub fixed on the model
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1896157\OneDrive - University of Edinburgh\Rafael\Models\MaxProfitFeeding\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="337">
   <si>
     <t>IFN</t>
   </si>
@@ -1016,9 +1016,6 @@
     <t>GSS</t>
   </si>
   <si>
-    <t>BF</t>
-  </si>
-  <si>
     <t>LB</t>
   </si>
   <si>
@@ -1035,6 +1032,12 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Sc1</t>
+  </si>
+  <si>
+    <t>Sc2</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1145,28 +1148,6 @@
       <top style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1192,7 +1173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
@@ -1221,19 +1202,32 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="77">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1531,17 +1525,50 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1648,17 +1675,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E13" totalsRowShown="0" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E13" totalsRowShown="0" dataDxfId="76">
   <autoFilter ref="A1:E13"/>
   <sortState ref="A2:E30">
     <sortCondition ref="A1:A30"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="68"/>
-    <tableColumn id="2" name="Min" dataDxfId="67"/>
-    <tableColumn id="3" name="Max" dataDxfId="66"/>
-    <tableColumn id="4" name="Cost" dataDxfId="65"/>
-    <tableColumn id="5" name="Name" dataDxfId="64">
+    <tableColumn id="1" name="ID" dataDxfId="75"/>
+    <tableColumn id="2" name="Min" dataDxfId="74"/>
+    <tableColumn id="3" name="Max" dataDxfId="73"/>
+    <tableColumn id="4" name="Cost" dataDxfId="72"/>
+    <tableColumn id="5" name="Name" dataDxfId="71">
       <calculatedColumnFormula>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1667,17 +1694,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="70" tableBorderDxfId="69">
   <autoFilter ref="A1:Q3"/>
   <tableColumns count="17">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Breed"/>
-    <tableColumn id="3" name="SBW"/>
-    <tableColumn id="4" name="BCS"/>
-    <tableColumn id="5" name="BE"/>
-    <tableColumn id="6" name="L"/>
-    <tableColumn id="7" name="SEX"/>
-    <tableColumn id="8" name="a2"/>
+    <tableColumn id="2" name="Breed" dataDxfId="68"/>
+    <tableColumn id="3" name="SBW" dataDxfId="67"/>
+    <tableColumn id="4" name="BCS" dataDxfId="66"/>
+    <tableColumn id="5" name="BE" dataDxfId="65"/>
+    <tableColumn id="6" name="L" dataDxfId="64"/>
+    <tableColumn id="7" name="SEX" dataDxfId="63"/>
+    <tableColumn id="8" name="a2" dataDxfId="62"/>
     <tableColumn id="9" name="PH"/>
     <tableColumn id="10" name="Selling Price"/>
     <tableColumn id="11" name="Linearization factor"/>
@@ -1693,70 +1720,70 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:BF219"/>
   <sortState ref="A2:BF219">
     <sortCondition ref="A4:A5"/>
   </sortState>
   <tableColumns count="58">
-    <tableColumn id="1" name="ID" dataDxfId="57"/>
-    <tableColumn id="2" name="Feed" dataDxfId="56"/>
-    <tableColumn id="4" name="IFN" dataDxfId="55"/>
-    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="54"/>
-    <tableColumn id="7" name="Forage, %DM" dataDxfId="53"/>
-    <tableColumn id="8" name="DM, %AF" dataDxfId="52"/>
-    <tableColumn id="16" name="CP, %DM" dataDxfId="51"/>
-    <tableColumn id="31" name="SP, %CP" dataDxfId="50"/>
-    <tableColumn id="29" name="ADICP, %CP" dataDxfId="49"/>
-    <tableColumn id="24" name="Sugars, %DM" dataDxfId="48"/>
-    <tableColumn id="25" name="OA, %DM" dataDxfId="47"/>
-    <tableColumn id="23" name="Fat, %DM" dataDxfId="46"/>
-    <tableColumn id="9" name="Ash, %DM" dataDxfId="45"/>
-    <tableColumn id="10" name="Starch, %DM" dataDxfId="44"/>
-    <tableColumn id="12" name="NDF, %DM" dataDxfId="43"/>
-    <tableColumn id="13" name="Lignin, %DM" dataDxfId="42"/>
-    <tableColumn id="14" name="TDN, %DM" dataDxfId="41"/>
-    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="40"/>
-    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="39"/>
-    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="38"/>
-    <tableColumn id="21" name="RUP, %CP" dataDxfId="37"/>
-    <tableColumn id="22" name="kd PB, %/h" dataDxfId="36"/>
-    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="35"/>
-    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="34"/>
-    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="33"/>
-    <tableColumn id="28" name="PBID, %" dataDxfId="32"/>
-    <tableColumn id="6" name="CB1ID, %" dataDxfId="31"/>
-    <tableColumn id="3" name="CB2ID, %" dataDxfId="30"/>
-    <tableColumn id="20" name="pef, %NDF" dataDxfId="29"/>
-    <tableColumn id="11" name="ARG, %DM" dataDxfId="28"/>
-    <tableColumn id="32" name="HIS, %DM" dataDxfId="27"/>
-    <tableColumn id="33" name="ILE, %DM" dataDxfId="26"/>
-    <tableColumn id="34" name="LEU, %DM" dataDxfId="25"/>
-    <tableColumn id="35" name="LYS, %DM" dataDxfId="24"/>
-    <tableColumn id="36" name="MET, %DM" dataDxfId="23"/>
-    <tableColumn id="37" name="CYS, %DM" dataDxfId="22"/>
-    <tableColumn id="38" name="PHE, %DM" dataDxfId="21"/>
-    <tableColumn id="39" name="TYR, %DM" dataDxfId="20"/>
-    <tableColumn id="40" name="THR, %DM" dataDxfId="19"/>
-    <tableColumn id="41" name="TRP, %DM" dataDxfId="18"/>
-    <tableColumn id="42" name="VAL, %DM" dataDxfId="17"/>
-    <tableColumn id="43" name="Ca, % DM" dataDxfId="16"/>
-    <tableColumn id="44" name="P, % DM" dataDxfId="15"/>
-    <tableColumn id="45" name="Mg, % DM" dataDxfId="14"/>
-    <tableColumn id="46" name="Cl, % DM" dataDxfId="13"/>
-    <tableColumn id="47" name="K, % DM" dataDxfId="12"/>
-    <tableColumn id="48" name="Na, % DM" dataDxfId="11"/>
-    <tableColumn id="49" name="S, % DM" dataDxfId="10"/>
-    <tableColumn id="50" name="Co, mg/kg" dataDxfId="9"/>
-    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="8"/>
-    <tableColumn id="52" name="I, mg/kg" dataDxfId="7"/>
-    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="6"/>
-    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="5"/>
-    <tableColumn id="55" name="Se, mg/kg" dataDxfId="4"/>
-    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="3"/>
-    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="2"/>
-    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="1"/>
-    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="59"/>
+    <tableColumn id="2" name="Feed" dataDxfId="58"/>
+    <tableColumn id="4" name="IFN" dataDxfId="57"/>
+    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="56"/>
+    <tableColumn id="7" name="Forage, %DM" dataDxfId="55"/>
+    <tableColumn id="8" name="DM, %AF" dataDxfId="54"/>
+    <tableColumn id="16" name="CP, %DM" dataDxfId="53"/>
+    <tableColumn id="31" name="SP, %CP" dataDxfId="52"/>
+    <tableColumn id="29" name="ADICP, %CP" dataDxfId="51"/>
+    <tableColumn id="24" name="Sugars, %DM" dataDxfId="50"/>
+    <tableColumn id="25" name="OA, %DM" dataDxfId="49"/>
+    <tableColumn id="23" name="Fat, %DM" dataDxfId="48"/>
+    <tableColumn id="9" name="Ash, %DM" dataDxfId="47"/>
+    <tableColumn id="10" name="Starch, %DM" dataDxfId="46"/>
+    <tableColumn id="12" name="NDF, %DM" dataDxfId="45"/>
+    <tableColumn id="13" name="Lignin, %DM" dataDxfId="44"/>
+    <tableColumn id="14" name="TDN, %DM" dataDxfId="43"/>
+    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="42"/>
+    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="41"/>
+    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="40"/>
+    <tableColumn id="21" name="RUP, %CP" dataDxfId="39"/>
+    <tableColumn id="22" name="kd PB, %/h" dataDxfId="38"/>
+    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="37"/>
+    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="36"/>
+    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="35"/>
+    <tableColumn id="28" name="PBID, %" dataDxfId="34"/>
+    <tableColumn id="6" name="CB1ID, %" dataDxfId="33"/>
+    <tableColumn id="3" name="CB2ID, %" dataDxfId="32"/>
+    <tableColumn id="20" name="pef, %NDF" dataDxfId="31"/>
+    <tableColumn id="11" name="ARG, %DM" dataDxfId="30"/>
+    <tableColumn id="32" name="HIS, %DM" dataDxfId="29"/>
+    <tableColumn id="33" name="ILE, %DM" dataDxfId="28"/>
+    <tableColumn id="34" name="LEU, %DM" dataDxfId="27"/>
+    <tableColumn id="35" name="LYS, %DM" dataDxfId="26"/>
+    <tableColumn id="36" name="MET, %DM" dataDxfId="25"/>
+    <tableColumn id="37" name="CYS, %DM" dataDxfId="24"/>
+    <tableColumn id="38" name="PHE, %DM" dataDxfId="23"/>
+    <tableColumn id="39" name="TYR, %DM" dataDxfId="22"/>
+    <tableColumn id="40" name="THR, %DM" dataDxfId="21"/>
+    <tableColumn id="41" name="TRP, %DM" dataDxfId="20"/>
+    <tableColumn id="42" name="VAL, %DM" dataDxfId="19"/>
+    <tableColumn id="43" name="Ca, % DM" dataDxfId="18"/>
+    <tableColumn id="44" name="P, % DM" dataDxfId="17"/>
+    <tableColumn id="45" name="Mg, % DM" dataDxfId="16"/>
+    <tableColumn id="46" name="Cl, % DM" dataDxfId="15"/>
+    <tableColumn id="47" name="K, % DM" dataDxfId="14"/>
+    <tableColumn id="48" name="Na, % DM" dataDxfId="13"/>
+    <tableColumn id="49" name="S, % DM" dataDxfId="12"/>
+    <tableColumn id="50" name="Co, mg/kg" dataDxfId="11"/>
+    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="10"/>
+    <tableColumn id="52" name="I, mg/kg" dataDxfId="9"/>
+    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="8"/>
+    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="7"/>
+    <tableColumn id="55" name="Se, mg/kg" dataDxfId="6"/>
+    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="5"/>
+    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="4"/>
+    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="3"/>
+    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2025,13 +2052,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2054,7 +2081,7 @@
         <v>314</v>
       </c>
       <c r="D1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E1" t="s">
         <v>325</v>
@@ -2068,7 +2095,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="17">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D2" s="18">
         <v>0.13888888888888887</v>
@@ -2086,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D3" s="18">
         <v>0.17676767676767677</v>
@@ -2104,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="20">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D4" s="21">
         <v>0.19</v>
@@ -2122,7 +2149,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D5" s="18">
         <v>0.33333333333333337</v>
@@ -2140,7 +2167,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D6" s="18">
         <v>0.11363636363636365</v>
@@ -2158,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D7" s="18">
         <v>0.14000000000000001</v>
@@ -2176,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D8" s="18">
         <v>0.10101010101010102</v>
@@ -2194,7 +2221,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D9" s="18">
         <v>0.16414141414141412</v>
@@ -2212,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D10" s="18">
         <v>0.19696969696969696</v>
@@ -2230,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D11" s="18">
         <v>8.8383838383838384E-2</v>
@@ -2248,7 +2275,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D12" s="18">
         <v>0.15151515151515152</v>
@@ -2266,7 +2293,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D13" s="18">
         <v>0.40404040404040409</v>
@@ -2286,13 +2313,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet2">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q13" sqref="O13:Q16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K14" sqref="K13:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,97 +2339,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>321</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q1" s="28" t="s">
         <v>333</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>327</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>326</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>330</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>331</v>
-      </c>
-      <c r="P1" s="28" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="24">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>318</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="23">
         <v>300</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="23">
         <v>5</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="23">
         <v>1</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="23">
         <v>1</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="23">
         <v>1</v>
       </c>
-      <c r="H2" s="24">
-        <v>0</v>
-      </c>
-      <c r="I2" s="24">
+      <c r="H2" s="23">
+        <v>0</v>
+      </c>
+      <c r="I2" s="23">
         <v>6.2</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="23">
         <v>1.44</v>
       </c>
-      <c r="K2" s="25">
-        <v>13.91</v>
+      <c r="K2" s="23">
+        <v>0.87</v>
       </c>
       <c r="L2" s="23" t="s">
         <v>328</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="N2" s="23">
         <v>0.8</v>
@@ -2413,60 +2440,60 @@
       <c r="P2" s="23">
         <v>1E-3</v>
       </c>
-      <c r="Q2" t="b">
+      <c r="Q2" s="23" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+      <c r="A3" s="27">
         <v>2</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="29">
-        <v>300</v>
-      </c>
-      <c r="D3" s="29">
+      <c r="C3" s="27">
+        <v>310</v>
+      </c>
+      <c r="D3" s="27">
         <v>5</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="27">
         <v>1</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="27">
         <v>1</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="27">
         <v>1</v>
       </c>
-      <c r="H3" s="29">
-        <v>0</v>
-      </c>
-      <c r="I3" s="29">
+      <c r="H3" s="27">
+        <v>0</v>
+      </c>
+      <c r="I3" s="27">
         <v>6.2</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="27">
         <v>1.44</v>
       </c>
-      <c r="K3" s="30">
-        <v>13.91</v>
-      </c>
-      <c r="L3" s="29" t="s">
-        <v>329</v>
-      </c>
-      <c r="M3" s="29" t="s">
-        <v>329</v>
-      </c>
-      <c r="N3" s="29">
+      <c r="K3" s="27">
+        <v>0.87</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="M3" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="N3" s="27">
         <v>0.8</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="27">
         <v>3</v>
       </c>
-      <c r="P3" s="29">
+      <c r="P3" s="27">
         <v>1E-3</v>
       </c>
-      <c r="Q3" t="b">
+      <c r="Q3" s="27" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2480,7 +2507,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="A1:BF219"/>
@@ -40731,10 +40758,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:BF219">
-    <cfRule type="expression" dxfId="61" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>ROW(A2)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>COLUMN(A2)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40748,6 +40775,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:A58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41061,6 +41089,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43da31f6e8d8dfaec40561525ce78865">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b58fc7e6f492e58d10793199fba37542" ns3:_="" ns4:_="">
     <xsd:import namespace="871f9270-bc3b-4105-9923-e7982e1cb312"/>
@@ -41263,25 +41300,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -41290,6 +41318,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE8DA1A1-DD54-4881-BC06-911C3C5870BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41306,12 +41342,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
New feature: You can create different feed scenarios, also bugs fixed
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1896157\OneDrive - University of Edinburgh\Rafael\Models\MaxProfitFeeding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1896157_ed_ac_uk/Documents/Rafael/Models/MaxProfitFeeding/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Feeds" sheetId="2" r:id="rId1"/>
@@ -26,8 +26,166 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>MARQUES Gabriel</author>
+  </authors>
+  <commentList>
+    <comment ref="E6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MARQUES Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0.11</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MARQUES Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0.14
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MARQUES Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0.1
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MARQUES Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0.11</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MARQUES Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0.14
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MARQUES Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0.1
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="374">
   <si>
     <t>IFN</t>
   </si>
@@ -1001,9 +1159,6 @@
     <t>PH</t>
   </si>
   <si>
-    <t>Selling Price</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -1011,9 +1166,6 @@
   </si>
   <si>
     <t>Algorithm</t>
-  </si>
-  <si>
-    <t>GSS</t>
   </si>
   <si>
     <t>LB</t>
@@ -1028,16 +1180,133 @@
     <t>Linearization factor</t>
   </si>
   <si>
-    <t>LCA</t>
+    <t>Obj</t>
   </si>
   <si>
-    <t>Cost</t>
+    <t>BF-Max</t>
   </si>
   <si>
-    <t>Sc1</t>
+    <t>MaxProfit</t>
   </si>
   <si>
-    <t>Sc2</t>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>GSS</t>
+  </si>
+  <si>
+    <t>Feed Scenario</t>
+  </si>
+  <si>
+    <t>Feed Scenario 2</t>
+  </si>
+  <si>
+    <t>BF-Min</t>
+  </si>
+  <si>
+    <t>MinCost</t>
+  </si>
+  <si>
+    <t>BF-MaxP per SWG</t>
+  </si>
+  <si>
+    <t>MaxProfitSWG</t>
+  </si>
+  <si>
+    <t>GSS-Max</t>
+  </si>
+  <si>
+    <t>GSS-Max(+5)</t>
+  </si>
+  <si>
+    <t>GSS-Max(+10)</t>
+  </si>
+  <si>
+    <t>GSS-Max(+15)</t>
+  </si>
+  <si>
+    <t>GSS-Max(-5)</t>
+  </si>
+  <si>
+    <t>GSS-Max(-10)</t>
+  </si>
+  <si>
+    <t>GSS-Max(-15)</t>
+  </si>
+  <si>
+    <t>GSS-Min</t>
+  </si>
+  <si>
+    <t>GSS-Min(+5)</t>
+  </si>
+  <si>
+    <t>GSS-Min(+10)</t>
+  </si>
+  <si>
+    <t>GSS-Min(+15)</t>
+  </si>
+  <si>
+    <t>GSS-Min(-5)</t>
+  </si>
+  <si>
+    <t>GSS-Min(-10)</t>
+  </si>
+  <si>
+    <t>GSS-Min(-15)</t>
+  </si>
+  <si>
+    <t>GSS-Max(W250)</t>
+  </si>
+  <si>
+    <t>GSS-Max(W275)</t>
+  </si>
+  <si>
+    <t>GSS-Max(W325)</t>
+  </si>
+  <si>
+    <t>GSS-Max(W350)</t>
+  </si>
+  <si>
+    <t>BCS3</t>
+  </si>
+  <si>
+    <t>BCS4</t>
+  </si>
+  <si>
+    <t>BCS6</t>
+  </si>
+  <si>
+    <t>BCS7</t>
+  </si>
+  <si>
+    <t>350-3-15+</t>
+  </si>
+  <si>
+    <t>350-7-15+</t>
+  </si>
+  <si>
+    <t>350-3-15-</t>
+  </si>
+  <si>
+    <t>350-7-15-</t>
+  </si>
+  <si>
+    <t>250-3-15+</t>
+  </si>
+  <si>
+    <t>250-7-15+</t>
+  </si>
+  <si>
+    <t>250-3-15-</t>
+  </si>
+  <si>
+    <t>250-7-15-</t>
+  </si>
+  <si>
+    <t>Cost [US$/kg AF]</t>
+  </si>
+  <si>
+    <t>Selling Price [US$]</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1317,7 @@
     <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
     <numFmt numFmtId="165" formatCode="0.00;0.00;0;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1064,8 +1333,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1090,20 +1372,8 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1142,38 +1412,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
@@ -1197,37 +1440,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="69">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1525,89 +1743,17 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1661,6 +1807,14 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1675,17 +1829,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E13" totalsRowShown="0" dataDxfId="76">
-  <autoFilter ref="A1:E13"/>
-  <sortState ref="A2:E30">
-    <sortCondition ref="A1:A30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F25" totalsRowShown="0" dataDxfId="68">
+  <autoFilter ref="A1:F25"/>
+  <sortState ref="B2:F30">
+    <sortCondition ref="B1:B30"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="75"/>
-    <tableColumn id="2" name="Min" dataDxfId="74"/>
-    <tableColumn id="3" name="Max" dataDxfId="73"/>
-    <tableColumn id="4" name="Cost" dataDxfId="72"/>
-    <tableColumn id="5" name="Name" dataDxfId="71">
+  <tableColumns count="6">
+    <tableColumn id="6" name="Feed Scenario" dataDxfId="67"/>
+    <tableColumn id="1" name="ID" dataDxfId="66"/>
+    <tableColumn id="2" name="Min" dataDxfId="65"/>
+    <tableColumn id="3" name="Max" dataDxfId="64"/>
+    <tableColumn id="4" name="Cost [US$/kg AF]" dataDxfId="63"/>
+    <tableColumn id="5" name="Name" dataDxfId="62">
       <calculatedColumnFormula>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1694,96 +1849,97 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q3" totalsRowShown="0" headerRowDxfId="70" tableBorderDxfId="69">
-  <autoFilter ref="A1:Q3"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Scenario" displayName="Scenario" ref="A1:R35" totalsRowShown="0">
+  <autoFilter ref="A1:R35"/>
+  <tableColumns count="18">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Breed" dataDxfId="68"/>
-    <tableColumn id="3" name="SBW" dataDxfId="67"/>
-    <tableColumn id="4" name="BCS" dataDxfId="66"/>
-    <tableColumn id="5" name="BE" dataDxfId="65"/>
-    <tableColumn id="6" name="L" dataDxfId="64"/>
-    <tableColumn id="7" name="SEX" dataDxfId="63"/>
-    <tableColumn id="8" name="a2" dataDxfId="62"/>
+    <tableColumn id="18" name="Feed Scenario"/>
+    <tableColumn id="2" name="Breed"/>
+    <tableColumn id="3" name="SBW"/>
+    <tableColumn id="4" name="BCS"/>
+    <tableColumn id="5" name="BE"/>
+    <tableColumn id="6" name="L"/>
+    <tableColumn id="7" name="SEX"/>
+    <tableColumn id="8" name="a2"/>
     <tableColumn id="9" name="PH"/>
-    <tableColumn id="10" name="Selling Price"/>
+    <tableColumn id="10" name="Selling Price [US$]"/>
     <tableColumn id="11" name="Linearization factor"/>
     <tableColumn id="12" name="Algorithm"/>
     <tableColumn id="13" name="Identifier"/>
     <tableColumn id="14" name="LB"/>
     <tableColumn id="15" name="UB"/>
     <tableColumn id="16" name="Tol"/>
-    <tableColumn id="17" name="LCA"/>
+    <tableColumn id="17" name="Obj"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A1:BF219"/>
   <sortState ref="A2:BF219">
     <sortCondition ref="A4:A5"/>
   </sortState>
   <tableColumns count="58">
-    <tableColumn id="1" name="ID" dataDxfId="59"/>
-    <tableColumn id="2" name="Feed" dataDxfId="58"/>
-    <tableColumn id="4" name="IFN" dataDxfId="57"/>
-    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="56"/>
-    <tableColumn id="7" name="Forage, %DM" dataDxfId="55"/>
-    <tableColumn id="8" name="DM, %AF" dataDxfId="54"/>
-    <tableColumn id="16" name="CP, %DM" dataDxfId="53"/>
-    <tableColumn id="31" name="SP, %CP" dataDxfId="52"/>
-    <tableColumn id="29" name="ADICP, %CP" dataDxfId="51"/>
-    <tableColumn id="24" name="Sugars, %DM" dataDxfId="50"/>
-    <tableColumn id="25" name="OA, %DM" dataDxfId="49"/>
-    <tableColumn id="23" name="Fat, %DM" dataDxfId="48"/>
-    <tableColumn id="9" name="Ash, %DM" dataDxfId="47"/>
-    <tableColumn id="10" name="Starch, %DM" dataDxfId="46"/>
-    <tableColumn id="12" name="NDF, %DM" dataDxfId="45"/>
-    <tableColumn id="13" name="Lignin, %DM" dataDxfId="44"/>
-    <tableColumn id="14" name="TDN, %DM" dataDxfId="43"/>
-    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="42"/>
-    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="41"/>
-    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="40"/>
-    <tableColumn id="21" name="RUP, %CP" dataDxfId="39"/>
-    <tableColumn id="22" name="kd PB, %/h" dataDxfId="38"/>
-    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="37"/>
-    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="36"/>
-    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="35"/>
-    <tableColumn id="28" name="PBID, %" dataDxfId="34"/>
-    <tableColumn id="6" name="CB1ID, %" dataDxfId="33"/>
-    <tableColumn id="3" name="CB2ID, %" dataDxfId="32"/>
-    <tableColumn id="20" name="pef, %NDF" dataDxfId="31"/>
-    <tableColumn id="11" name="ARG, %DM" dataDxfId="30"/>
-    <tableColumn id="32" name="HIS, %DM" dataDxfId="29"/>
-    <tableColumn id="33" name="ILE, %DM" dataDxfId="28"/>
-    <tableColumn id="34" name="LEU, %DM" dataDxfId="27"/>
-    <tableColumn id="35" name="LYS, %DM" dataDxfId="26"/>
-    <tableColumn id="36" name="MET, %DM" dataDxfId="25"/>
-    <tableColumn id="37" name="CYS, %DM" dataDxfId="24"/>
-    <tableColumn id="38" name="PHE, %DM" dataDxfId="23"/>
-    <tableColumn id="39" name="TYR, %DM" dataDxfId="22"/>
-    <tableColumn id="40" name="THR, %DM" dataDxfId="21"/>
-    <tableColumn id="41" name="TRP, %DM" dataDxfId="20"/>
-    <tableColumn id="42" name="VAL, %DM" dataDxfId="19"/>
-    <tableColumn id="43" name="Ca, % DM" dataDxfId="18"/>
-    <tableColumn id="44" name="P, % DM" dataDxfId="17"/>
-    <tableColumn id="45" name="Mg, % DM" dataDxfId="16"/>
-    <tableColumn id="46" name="Cl, % DM" dataDxfId="15"/>
-    <tableColumn id="47" name="K, % DM" dataDxfId="14"/>
-    <tableColumn id="48" name="Na, % DM" dataDxfId="13"/>
-    <tableColumn id="49" name="S, % DM" dataDxfId="12"/>
-    <tableColumn id="50" name="Co, mg/kg" dataDxfId="11"/>
-    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="10"/>
-    <tableColumn id="52" name="I, mg/kg" dataDxfId="9"/>
-    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="8"/>
-    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="7"/>
-    <tableColumn id="55" name="Se, mg/kg" dataDxfId="6"/>
-    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="5"/>
-    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="4"/>
-    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="3"/>
-    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="2"/>
+    <tableColumn id="1" name="ID" dataDxfId="57"/>
+    <tableColumn id="2" name="Feed" dataDxfId="56"/>
+    <tableColumn id="4" name="IFN" dataDxfId="55"/>
+    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="54"/>
+    <tableColumn id="7" name="Forage, %DM" dataDxfId="53"/>
+    <tableColumn id="8" name="DM, %AF" dataDxfId="52"/>
+    <tableColumn id="16" name="CP, %DM" dataDxfId="51"/>
+    <tableColumn id="31" name="SP, %CP" dataDxfId="50"/>
+    <tableColumn id="29" name="ADICP, %CP" dataDxfId="49"/>
+    <tableColumn id="24" name="Sugars, %DM" dataDxfId="48"/>
+    <tableColumn id="25" name="OA, %DM" dataDxfId="47"/>
+    <tableColumn id="23" name="Fat, %DM" dataDxfId="46"/>
+    <tableColumn id="9" name="Ash, %DM" dataDxfId="45"/>
+    <tableColumn id="10" name="Starch, %DM" dataDxfId="44"/>
+    <tableColumn id="12" name="NDF, %DM" dataDxfId="43"/>
+    <tableColumn id="13" name="Lignin, %DM" dataDxfId="42"/>
+    <tableColumn id="14" name="TDN, %DM" dataDxfId="41"/>
+    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="40"/>
+    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="39"/>
+    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="38"/>
+    <tableColumn id="21" name="RUP, %CP" dataDxfId="37"/>
+    <tableColumn id="22" name="kd PB, %/h" dataDxfId="36"/>
+    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="35"/>
+    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="34"/>
+    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="33"/>
+    <tableColumn id="28" name="PBID, %" dataDxfId="32"/>
+    <tableColumn id="6" name="CB1ID, %" dataDxfId="31"/>
+    <tableColumn id="3" name="CB2ID, %" dataDxfId="30"/>
+    <tableColumn id="20" name="pef, %NDF" dataDxfId="29"/>
+    <tableColumn id="11" name="ARG, %DM" dataDxfId="28"/>
+    <tableColumn id="32" name="HIS, %DM" dataDxfId="27"/>
+    <tableColumn id="33" name="ILE, %DM" dataDxfId="26"/>
+    <tableColumn id="34" name="LEU, %DM" dataDxfId="25"/>
+    <tableColumn id="35" name="LYS, %DM" dataDxfId="24"/>
+    <tableColumn id="36" name="MET, %DM" dataDxfId="23"/>
+    <tableColumn id="37" name="CYS, %DM" dataDxfId="22"/>
+    <tableColumn id="38" name="PHE, %DM" dataDxfId="21"/>
+    <tableColumn id="39" name="TYR, %DM" dataDxfId="20"/>
+    <tableColumn id="40" name="THR, %DM" dataDxfId="19"/>
+    <tableColumn id="41" name="TRP, %DM" dataDxfId="18"/>
+    <tableColumn id="42" name="VAL, %DM" dataDxfId="17"/>
+    <tableColumn id="43" name="Ca, % DM" dataDxfId="16"/>
+    <tableColumn id="44" name="P, % DM" dataDxfId="15"/>
+    <tableColumn id="45" name="Mg, % DM" dataDxfId="14"/>
+    <tableColumn id="46" name="Cl, % DM" dataDxfId="13"/>
+    <tableColumn id="47" name="K, % DM" dataDxfId="12"/>
+    <tableColumn id="48" name="Na, % DM" dataDxfId="11"/>
+    <tableColumn id="49" name="S, % DM" dataDxfId="10"/>
+    <tableColumn id="50" name="Co, mg/kg" dataDxfId="9"/>
+    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="8"/>
+    <tableColumn id="52" name="I, mg/kg" dataDxfId="7"/>
+    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="6"/>
+    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="5"/>
+    <tableColumn id="55" name="Se, mg/kg" dataDxfId="4"/>
+    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="3"/>
+    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="2"/>
+    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="1"/>
+    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2051,14 +2207,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,245 +2224,538 @@
     <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>313</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>314</v>
       </c>
-      <c r="D1" t="s">
-        <v>334</v>
-      </c>
       <c r="E1" t="s">
-        <v>325</v>
+        <v>372</v>
+      </c>
+      <c r="F1" t="s">
+        <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16">
         <v>34</v>
       </c>
-      <c r="B2" s="17">
-        <v>0</v>
-      </c>
       <c r="C2" s="17">
-        <v>2</v>
-      </c>
-      <c r="D2" s="18">
+        <v>0</v>
+      </c>
+      <c r="D2" s="17">
+        <v>1</v>
+      </c>
+      <c r="E2" s="18">
         <v>0.13888888888888887</v>
       </c>
-      <c r="E2" s="17" t="str">
+      <c r="F2" s="17" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Citrus pulp, dry</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16">
         <v>45</v>
       </c>
-      <c r="B3" s="17">
-        <v>0</v>
-      </c>
       <c r="C3" s="17">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17">
         <v>1</v>
       </c>
-      <c r="D3" s="18">
+      <c r="E3" s="18">
         <v>0.17676767676767677</v>
       </c>
-      <c r="E3" s="17" t="str">
+      <c r="F3" s="17" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Corn grain</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="16">
         <v>50</v>
       </c>
-      <c r="B4" s="20">
-        <v>0</v>
-      </c>
-      <c r="C4" s="20">
+      <c r="C4" s="17">
+        <v>0</v>
+      </c>
+      <c r="D4" s="17">
         <v>1</v>
       </c>
-      <c r="D4" s="21">
+      <c r="E4" s="18">
         <v>0.19</v>
       </c>
-      <c r="E4" s="22" t="str">
+      <c r="F4" s="19" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Corn silage</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="17">
         <v>58</v>
       </c>
-      <c r="B5" s="17">
-        <v>0</v>
-      </c>
       <c r="C5" s="17">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17">
         <v>1</v>
       </c>
-      <c r="D5" s="18">
+      <c r="E5" s="18">
         <v>0.33333333333333337</v>
       </c>
-      <c r="E5" s="17" t="str">
+      <c r="F5" s="17" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Cottonseed meal</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="17">
         <v>59</v>
       </c>
-      <c r="B6" s="17">
-        <v>0</v>
-      </c>
       <c r="C6" s="17">
+        <v>0</v>
+      </c>
+      <c r="D6" s="17">
         <v>1</v>
       </c>
-      <c r="D6" s="18">
-        <v>0.11363636363636365</v>
-      </c>
-      <c r="E6" s="17" t="str">
+      <c r="E6" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F6" s="17" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Cottonseed whole</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="17">
         <v>60</v>
       </c>
-      <c r="B7" s="17">
-        <v>0</v>
-      </c>
       <c r="C7" s="17">
+        <v>0</v>
+      </c>
+      <c r="D7" s="17">
         <v>1</v>
       </c>
-      <c r="D7" s="18">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E7" s="17" t="str">
+      <c r="E7" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="F7" s="17" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Distillers grain plus soluble, dry</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="17">
         <v>79</v>
       </c>
-      <c r="B8" s="17">
-        <v>0</v>
-      </c>
       <c r="C8" s="17">
+        <v>0</v>
+      </c>
+      <c r="D8" s="17">
         <v>1</v>
       </c>
-      <c r="D8" s="18">
-        <v>0.10101010101010102</v>
-      </c>
-      <c r="E8" s="17" t="str">
+      <c r="E8" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F8" s="17" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Grain sorghum grain</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="17">
         <v>133</v>
       </c>
-      <c r="B9" s="17">
-        <v>0</v>
-      </c>
       <c r="C9" s="17">
+        <v>0</v>
+      </c>
+      <c r="D9" s="17">
         <v>1</v>
       </c>
-      <c r="D9" s="18">
+      <c r="E9" s="18">
         <v>0.16414141414141412</v>
       </c>
-      <c r="E9" s="17" t="str">
+      <c r="F9" s="17" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Soybean hulls</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="17">
         <v>134</v>
       </c>
-      <c r="B10" s="17">
-        <v>0</v>
-      </c>
       <c r="C10" s="17">
+        <v>0</v>
+      </c>
+      <c r="D10" s="17">
         <v>1</v>
       </c>
-      <c r="D10" s="18">
+      <c r="E10" s="18">
         <v>0.19696969696969696</v>
       </c>
-      <c r="E10" s="17" t="str">
+      <c r="F10" s="17" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Soybean meal high CP</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="17">
         <v>148</v>
       </c>
-      <c r="B11" s="17">
-        <v>0</v>
-      </c>
       <c r="C11" s="17">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17">
         <v>1</v>
       </c>
-      <c r="D11" s="18">
+      <c r="E11" s="18">
         <v>8.8383838383838384E-2</v>
       </c>
-      <c r="E11" s="17" t="str">
+      <c r="F11" s="17" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Sugarcane silage</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="17">
         <v>166</v>
       </c>
-      <c r="B12" s="17">
-        <v>0</v>
-      </c>
       <c r="C12" s="17">
+        <v>0</v>
+      </c>
+      <c r="D12" s="17">
         <v>1</v>
       </c>
-      <c r="D12" s="18">
+      <c r="E12" s="18">
         <v>0.15151515151515152</v>
       </c>
-      <c r="E12" s="17" t="str">
+      <c r="F12" s="17" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Wheat middlings</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="16">
         <v>845</v>
       </c>
-      <c r="B13" s="17">
-        <v>0</v>
-      </c>
       <c r="C13" s="17">
+        <v>0</v>
+      </c>
+      <c r="D13" s="17">
         <v>1</v>
       </c>
-      <c r="D13" s="18">
+      <c r="E13" s="18">
         <v>0.40404040404040409</v>
       </c>
-      <c r="E13" s="17" t="str">
+      <c r="F13" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Urea</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="16">
+        <v>34</v>
+      </c>
+      <c r="C14" s="17">
+        <v>0</v>
+      </c>
+      <c r="D14" s="17">
+        <v>1</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0.19</v>
+      </c>
+      <c r="F14" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Citrus pulp, dry</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="16">
+        <v>45</v>
+      </c>
+      <c r="C15" s="17">
+        <v>0</v>
+      </c>
+      <c r="D15" s="17">
+        <v>1</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="F15" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Corn grain</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" s="16">
+        <v>50</v>
+      </c>
+      <c r="C16" s="17">
+        <v>0</v>
+      </c>
+      <c r="D16" s="17">
+        <v>1</v>
+      </c>
+      <c r="E16" s="18">
+        <v>0.19</v>
+      </c>
+      <c r="F16" s="19" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Corn silage</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="17">
+        <v>58</v>
+      </c>
+      <c r="C17" s="17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="F17" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Cottonseed meal</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="17">
+        <v>59</v>
+      </c>
+      <c r="C18" s="17">
+        <v>0</v>
+      </c>
+      <c r="D18" s="17">
+        <v>1</v>
+      </c>
+      <c r="E18" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F18" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Cottonseed whole</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" s="17">
+        <v>60</v>
+      </c>
+      <c r="C19" s="17">
+        <v>0</v>
+      </c>
+      <c r="D19" s="17">
+        <v>1</v>
+      </c>
+      <c r="E19" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="F19" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Distillers grain plus soluble, dry</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" s="17">
+        <v>79</v>
+      </c>
+      <c r="C20" s="17">
+        <v>0</v>
+      </c>
+      <c r="D20" s="17">
+        <v>1</v>
+      </c>
+      <c r="E20" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F20" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Grain sorghum grain</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="17">
+        <v>133</v>
+      </c>
+      <c r="C21" s="17">
+        <v>0</v>
+      </c>
+      <c r="D21" s="17">
+        <v>1</v>
+      </c>
+      <c r="E21" s="18">
+        <v>0.16414141414141412</v>
+      </c>
+      <c r="F21" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Soybean hulls</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="17">
+        <v>134</v>
+      </c>
+      <c r="C22" s="17">
+        <v>0</v>
+      </c>
+      <c r="D22" s="17">
+        <v>1</v>
+      </c>
+      <c r="E22" s="18">
+        <v>0.19696969696969696</v>
+      </c>
+      <c r="F22" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Soybean meal high CP</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="17">
+        <v>148</v>
+      </c>
+      <c r="C23" s="17">
+        <v>0</v>
+      </c>
+      <c r="D23" s="17">
+        <v>1</v>
+      </c>
+      <c r="E23" s="18">
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="F23" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Sugarcane silage</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="17">
+        <v>166</v>
+      </c>
+      <c r="C24" s="17">
+        <v>0</v>
+      </c>
+      <c r="D24" s="17">
+        <v>1</v>
+      </c>
+      <c r="E24" s="18">
+        <v>0.40404040404040409</v>
+      </c>
+      <c r="F24" s="17" t="str">
+        <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
+        <v>Wheat middlings</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>2</v>
+      </c>
+      <c r="B25" s="16">
+        <v>845</v>
+      </c>
+      <c r="C25" s="17">
+        <v>0</v>
+      </c>
+      <c r="D25" s="17">
+        <v>1</v>
+      </c>
+      <c r="E25" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="F25" s="19" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</f>
         <v>Urea</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2316,185 +2765,2000 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K14" sqref="K13:K14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1" t="s">
         <v>315</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" t="s">
         <v>316</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="E1" t="s">
         <v>317</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" t="s">
         <v>319</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="G1" t="s">
         <v>320</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="H1" t="s">
         <v>321</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" t="s">
         <v>322</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" t="s">
         <v>323</v>
       </c>
-      <c r="J1" s="24" t="s">
-        <v>324</v>
-      </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" t="s">
+        <v>373</v>
+      </c>
+      <c r="L1" t="s">
+        <v>330</v>
+      </c>
+      <c r="M1" t="s">
+        <v>326</v>
+      </c>
+      <c r="N1" t="s">
+        <v>325</v>
+      </c>
+      <c r="O1" t="s">
+        <v>327</v>
+      </c>
+      <c r="P1" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>329</v>
+      </c>
+      <c r="R1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2">
+        <v>300</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>6.2</v>
+      </c>
+      <c r="K2">
+        <v>1.44</v>
+      </c>
+      <c r="L2">
+        <v>0.87</v>
+      </c>
+      <c r="M2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N2" t="s">
+        <v>338</v>
+      </c>
+      <c r="O2">
+        <v>0.8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>0.01</v>
+      </c>
+      <c r="R2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D3">
+        <v>300</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>6.2</v>
+      </c>
+      <c r="K3">
+        <v>1.44</v>
+      </c>
+      <c r="L3">
+        <v>0.87</v>
+      </c>
+      <c r="M3" t="s">
+        <v>334</v>
+      </c>
+      <c r="N3" t="s">
         <v>332</v>
       </c>
-      <c r="L1" s="26" t="s">
-        <v>327</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>326</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>329</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>330</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q1" s="28" t="s">
+      <c r="O3">
+        <v>0.8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>0.01</v>
+      </c>
+      <c r="R3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="C4" t="s">
         <v>318</v>
       </c>
-      <c r="C2" s="23">
+      <c r="D4">
         <v>300</v>
       </c>
-      <c r="D2" s="23">
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="E2" s="23">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="F2" s="23">
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="G2" s="23">
+      <c r="H4">
         <v>1</v>
       </c>
-      <c r="H2" s="23">
-        <v>0</v>
-      </c>
-      <c r="I2" s="23">
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>6.2</v>
       </c>
-      <c r="J2" s="23">
+      <c r="K4">
         <v>1.44</v>
       </c>
-      <c r="K2" s="23">
+      <c r="L4">
         <v>0.87</v>
       </c>
-      <c r="L2" s="23" t="s">
-        <v>328</v>
-      </c>
-      <c r="M2" s="23" t="s">
+      <c r="M4" t="s">
+        <v>334</v>
+      </c>
+      <c r="N4" t="s">
+        <v>340</v>
+      </c>
+      <c r="O4">
+        <v>0.8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>0.01</v>
+      </c>
+      <c r="R4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D5">
+        <v>300</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>6.2</v>
+      </c>
+      <c r="K5">
+        <v>1.44</v>
+      </c>
+      <c r="L5">
+        <v>0.87</v>
+      </c>
+      <c r="M5" t="s">
         <v>335</v>
       </c>
-      <c r="N2" s="23">
+      <c r="N5" t="s">
+        <v>342</v>
+      </c>
+      <c r="O5">
         <v>0.8</v>
       </c>
-      <c r="O2" s="23">
+      <c r="P5">
         <v>3</v>
       </c>
-      <c r="P2" s="23">
-        <v>1E-3</v>
-      </c>
-      <c r="Q2" s="23" t="b">
-        <v>0</v>
+      <c r="Q5">
+        <v>0.01</v>
+      </c>
+      <c r="R5" t="s">
+        <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="27">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>6.2</v>
+      </c>
+      <c r="K6">
+        <f>K5*1.05</f>
+        <v>1.512</v>
+      </c>
+      <c r="L6">
+        <v>0.87</v>
+      </c>
+      <c r="M6" t="s">
+        <v>335</v>
+      </c>
+      <c r="N6" t="s">
+        <v>343</v>
+      </c>
+      <c r="O6">
+        <v>0.8</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <v>0.01</v>
+      </c>
+      <c r="R6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7">
+        <v>300</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>6.2</v>
+      </c>
+      <c r="K7">
+        <f>K5*1.1</f>
+        <v>1.5840000000000001</v>
+      </c>
+      <c r="L7">
+        <v>0.87</v>
+      </c>
+      <c r="M7" t="s">
+        <v>335</v>
+      </c>
+      <c r="N7" t="s">
+        <v>344</v>
+      </c>
+      <c r="O7">
+        <v>0.8</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>0.01</v>
+      </c>
+      <c r="R7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>6.2</v>
+      </c>
+      <c r="K8">
+        <f>K5*1.15</f>
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="L8">
+        <v>0.87</v>
+      </c>
+      <c r="M8" t="s">
+        <v>335</v>
+      </c>
+      <c r="N8" t="s">
+        <v>345</v>
+      </c>
+      <c r="O8">
+        <v>0.8</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <v>0.01</v>
+      </c>
+      <c r="R8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9">
+        <v>300</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>6.2</v>
+      </c>
+      <c r="K9">
+        <f>K5*0.95</f>
+        <v>1.3679999999999999</v>
+      </c>
+      <c r="L9">
+        <v>0.87</v>
+      </c>
+      <c r="M9" t="s">
+        <v>335</v>
+      </c>
+      <c r="N9" t="s">
+        <v>346</v>
+      </c>
+      <c r="O9">
+        <v>0.8</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="Q9">
+        <v>0.01</v>
+      </c>
+      <c r="R9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10">
+        <v>300</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>6.2</v>
+      </c>
+      <c r="K10">
+        <f>K5*0.9</f>
+        <v>1.296</v>
+      </c>
+      <c r="L10">
+        <v>0.87</v>
+      </c>
+      <c r="M10" t="s">
+        <v>335</v>
+      </c>
+      <c r="N10" t="s">
+        <v>347</v>
+      </c>
+      <c r="O10">
+        <v>0.8</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>0.01</v>
+      </c>
+      <c r="R10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>318</v>
+      </c>
+      <c r="D11">
+        <v>300</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>6.2</v>
+      </c>
+      <c r="K11">
+        <f>K5*0.85</f>
+        <v>1.224</v>
+      </c>
+      <c r="L11">
+        <v>0.87</v>
+      </c>
+      <c r="M11" t="s">
+        <v>335</v>
+      </c>
+      <c r="N11" t="s">
+        <v>348</v>
+      </c>
+      <c r="O11">
+        <v>0.8</v>
+      </c>
+      <c r="P11">
+        <v>3</v>
+      </c>
+      <c r="Q11">
+        <v>0.01</v>
+      </c>
+      <c r="R11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12">
+        <v>300</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>6.2</v>
+      </c>
+      <c r="K12">
+        <v>1.44</v>
+      </c>
+      <c r="L12">
+        <v>0.87</v>
+      </c>
+      <c r="M12" t="s">
+        <v>335</v>
+      </c>
+      <c r="N12" t="s">
+        <v>349</v>
+      </c>
+      <c r="O12">
+        <v>0.8</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>0.01</v>
+      </c>
+      <c r="R12" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>318</v>
+      </c>
+      <c r="D13">
+        <v>300</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>6.2</v>
+      </c>
+      <c r="K13">
+        <f>K12*1.05</f>
+        <v>1.512</v>
+      </c>
+      <c r="L13">
+        <v>0.87</v>
+      </c>
+      <c r="M13" t="s">
+        <v>335</v>
+      </c>
+      <c r="N13" t="s">
+        <v>350</v>
+      </c>
+      <c r="O13">
+        <v>0.8</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+      <c r="Q13">
+        <v>0.01</v>
+      </c>
+      <c r="R13" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>318</v>
+      </c>
+      <c r="D14">
+        <v>300</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>6.2</v>
+      </c>
+      <c r="K14">
+        <f>K12*1.1</f>
+        <v>1.5840000000000001</v>
+      </c>
+      <c r="L14">
+        <v>0.87</v>
+      </c>
+      <c r="M14" t="s">
+        <v>335</v>
+      </c>
+      <c r="N14" t="s">
+        <v>351</v>
+      </c>
+      <c r="O14">
+        <v>0.8</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <v>0.01</v>
+      </c>
+      <c r="R14" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D15">
+        <v>300</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>6.2</v>
+      </c>
+      <c r="K15">
+        <f>K12*1.15</f>
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="L15">
+        <v>0.87</v>
+      </c>
+      <c r="M15" t="s">
+        <v>335</v>
+      </c>
+      <c r="N15" t="s">
+        <v>352</v>
+      </c>
+      <c r="O15">
+        <v>0.8</v>
+      </c>
+      <c r="P15">
+        <v>3</v>
+      </c>
+      <c r="Q15">
+        <v>0.01</v>
+      </c>
+      <c r="R15" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>318</v>
+      </c>
+      <c r="D16">
+        <v>300</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>6.2</v>
+      </c>
+      <c r="K16">
+        <f>K12*0.95</f>
+        <v>1.3679999999999999</v>
+      </c>
+      <c r="L16">
+        <v>0.87</v>
+      </c>
+      <c r="M16" t="s">
+        <v>335</v>
+      </c>
+      <c r="N16" t="s">
+        <v>353</v>
+      </c>
+      <c r="O16">
+        <v>0.8</v>
+      </c>
+      <c r="P16">
+        <v>3</v>
+      </c>
+      <c r="Q16">
+        <v>0.01</v>
+      </c>
+      <c r="R16" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>318</v>
+      </c>
+      <c r="D17">
+        <v>300</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>6.2</v>
+      </c>
+      <c r="K17">
+        <f>K12*0.9</f>
+        <v>1.296</v>
+      </c>
+      <c r="L17">
+        <v>0.87</v>
+      </c>
+      <c r="M17" t="s">
+        <v>335</v>
+      </c>
+      <c r="N17" t="s">
+        <v>354</v>
+      </c>
+      <c r="O17">
+        <v>0.8</v>
+      </c>
+      <c r="P17">
+        <v>3</v>
+      </c>
+      <c r="Q17">
+        <v>0.01</v>
+      </c>
+      <c r="R17" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>318</v>
+      </c>
+      <c r="D18">
+        <v>300</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>6.2</v>
+      </c>
+      <c r="K18">
+        <f>K12*0.85</f>
+        <v>1.224</v>
+      </c>
+      <c r="L18">
+        <v>0.87</v>
+      </c>
+      <c r="M18" t="s">
+        <v>335</v>
+      </c>
+      <c r="N18" t="s">
+        <v>355</v>
+      </c>
+      <c r="O18">
+        <v>0.8</v>
+      </c>
+      <c r="P18">
+        <v>3</v>
+      </c>
+      <c r="Q18">
+        <v>0.01</v>
+      </c>
+      <c r="R18" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>318</v>
+      </c>
+      <c r="D19">
+        <v>250</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>6.2</v>
+      </c>
+      <c r="K19">
+        <v>1.44</v>
+      </c>
+      <c r="L19">
+        <v>0.87</v>
+      </c>
+      <c r="M19" t="s">
+        <v>335</v>
+      </c>
+      <c r="N19" t="s">
+        <v>356</v>
+      </c>
+      <c r="O19">
+        <v>0.8</v>
+      </c>
+      <c r="P19">
+        <v>3</v>
+      </c>
+      <c r="Q19">
+        <v>0.01</v>
+      </c>
+      <c r="R19" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>318</v>
+      </c>
+      <c r="D20">
+        <v>275</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>6.2</v>
+      </c>
+      <c r="K20">
+        <v>1.44</v>
+      </c>
+      <c r="L20">
+        <v>0.87</v>
+      </c>
+      <c r="M20" t="s">
+        <v>335</v>
+      </c>
+      <c r="N20" t="s">
+        <v>357</v>
+      </c>
+      <c r="O20">
+        <v>0.8</v>
+      </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="Q20">
+        <v>0.01</v>
+      </c>
+      <c r="R20" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>318</v>
+      </c>
+      <c r="D21">
+        <v>325</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>6.2</v>
+      </c>
+      <c r="K21">
+        <v>1.44</v>
+      </c>
+      <c r="L21">
+        <v>0.87</v>
+      </c>
+      <c r="M21" t="s">
+        <v>335</v>
+      </c>
+      <c r="N21" t="s">
+        <v>358</v>
+      </c>
+      <c r="O21">
+        <v>0.8</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
+      </c>
+      <c r="Q21">
+        <v>0.01</v>
+      </c>
+      <c r="R21" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>318</v>
+      </c>
+      <c r="D22">
+        <v>350</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>6.2</v>
+      </c>
+      <c r="K22">
+        <v>1.44</v>
+      </c>
+      <c r="L22">
+        <v>0.87</v>
+      </c>
+      <c r="M22" t="s">
+        <v>335</v>
+      </c>
+      <c r="N22" t="s">
+        <v>359</v>
+      </c>
+      <c r="O22">
+        <v>0.8</v>
+      </c>
+      <c r="P22">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <v>0.01</v>
+      </c>
+      <c r="R22" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>318</v>
+      </c>
+      <c r="D23">
+        <v>300</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>6.2</v>
+      </c>
+      <c r="K23">
+        <v>1.44</v>
+      </c>
+      <c r="L23">
+        <v>0.87</v>
+      </c>
+      <c r="M23" t="s">
+        <v>335</v>
+      </c>
+      <c r="N23" t="s">
+        <v>360</v>
+      </c>
+      <c r="O23">
+        <v>0.8</v>
+      </c>
+      <c r="P23">
+        <v>3</v>
+      </c>
+      <c r="Q23">
+        <v>0.01</v>
+      </c>
+      <c r="R23" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>318</v>
+      </c>
+      <c r="D24">
+        <v>300</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>6.2</v>
+      </c>
+      <c r="K24">
+        <v>1.44</v>
+      </c>
+      <c r="L24">
+        <v>0.87</v>
+      </c>
+      <c r="M24" t="s">
+        <v>335</v>
+      </c>
+      <c r="N24" t="s">
+        <v>361</v>
+      </c>
+      <c r="O24">
+        <v>0.8</v>
+      </c>
+      <c r="P24">
+        <v>3</v>
+      </c>
+      <c r="Q24">
+        <v>0.01</v>
+      </c>
+      <c r="R24" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>318</v>
+      </c>
+      <c r="D25">
+        <v>300</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>6.2</v>
+      </c>
+      <c r="K25">
+        <v>1.44</v>
+      </c>
+      <c r="L25">
+        <v>0.87</v>
+      </c>
+      <c r="M25" t="s">
+        <v>335</v>
+      </c>
+      <c r="N25" t="s">
+        <v>362</v>
+      </c>
+      <c r="O25">
+        <v>0.8</v>
+      </c>
+      <c r="P25">
+        <v>3</v>
+      </c>
+      <c r="Q25">
+        <v>0.01</v>
+      </c>
+      <c r="R25" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>318</v>
+      </c>
+      <c r="D26">
+        <v>300</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>6.2</v>
+      </c>
+      <c r="K26">
+        <v>1.44</v>
+      </c>
+      <c r="L26">
+        <v>0.87</v>
+      </c>
+      <c r="M26" t="s">
+        <v>335</v>
+      </c>
+      <c r="N26" t="s">
+        <v>363</v>
+      </c>
+      <c r="O26">
+        <v>0.8</v>
+      </c>
+      <c r="P26">
+        <v>3</v>
+      </c>
+      <c r="Q26">
+        <v>0.01</v>
+      </c>
+      <c r="R26" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>318</v>
+      </c>
+      <c r="D27">
+        <v>350</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>6.2</v>
+      </c>
+      <c r="K27">
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="L27">
+        <v>0.87</v>
+      </c>
+      <c r="M27" t="s">
+        <v>335</v>
+      </c>
+      <c r="N27" t="s">
+        <v>364</v>
+      </c>
+      <c r="O27">
+        <v>0.8</v>
+      </c>
+      <c r="P27">
+        <v>3</v>
+      </c>
+      <c r="Q27">
+        <v>0.01</v>
+      </c>
+      <c r="R27" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>318</v>
+      </c>
+      <c r="D28">
+        <v>350</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>6.2</v>
+      </c>
+      <c r="K28">
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="L28">
+        <v>0.87</v>
+      </c>
+      <c r="M28" t="s">
+        <v>335</v>
+      </c>
+      <c r="N28" t="s">
+        <v>365</v>
+      </c>
+      <c r="O28">
+        <v>0.8</v>
+      </c>
+      <c r="P28">
+        <v>3</v>
+      </c>
+      <c r="Q28">
+        <v>0.01</v>
+      </c>
+      <c r="R28" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>318</v>
+      </c>
+      <c r="D29">
+        <v>350</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>6.2</v>
+      </c>
+      <c r="K29">
+        <v>1.224</v>
+      </c>
+      <c r="L29">
+        <v>0.87</v>
+      </c>
+      <c r="M29" t="s">
+        <v>335</v>
+      </c>
+      <c r="N29" t="s">
+        <v>366</v>
+      </c>
+      <c r="O29">
+        <v>0.8</v>
+      </c>
+      <c r="P29">
+        <v>3</v>
+      </c>
+      <c r="Q29">
+        <v>0.01</v>
+      </c>
+      <c r="R29" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>318</v>
+      </c>
+      <c r="D30">
+        <v>350</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>6.2</v>
+      </c>
+      <c r="K30">
+        <v>1.224</v>
+      </c>
+      <c r="L30">
+        <v>0.87</v>
+      </c>
+      <c r="M30" t="s">
+        <v>335</v>
+      </c>
+      <c r="N30" t="s">
+        <v>367</v>
+      </c>
+      <c r="O30">
+        <v>0.8</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
+      <c r="Q30">
+        <v>0.01</v>
+      </c>
+      <c r="R30" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>318</v>
+      </c>
+      <c r="D31">
+        <v>250</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>6.2</v>
+      </c>
+      <c r="K31">
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="L31">
+        <v>0.87</v>
+      </c>
+      <c r="M31" t="s">
+        <v>335</v>
+      </c>
+      <c r="N31" t="s">
+        <v>368</v>
+      </c>
+      <c r="O31">
+        <v>0.8</v>
+      </c>
+      <c r="P31">
+        <v>3</v>
+      </c>
+      <c r="Q31">
+        <v>0.01</v>
+      </c>
+      <c r="R31" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>318</v>
+      </c>
+      <c r="D32">
+        <v>250</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>6.2</v>
+      </c>
+      <c r="K32">
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="L32">
+        <v>0.87</v>
+      </c>
+      <c r="M32" t="s">
+        <v>335</v>
+      </c>
+      <c r="N32" t="s">
+        <v>369</v>
+      </c>
+      <c r="O32">
+        <v>0.8</v>
+      </c>
+      <c r="P32">
+        <v>3</v>
+      </c>
+      <c r="Q32">
+        <v>0.01</v>
+      </c>
+      <c r="R32" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D33">
+        <v>250</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>6.2</v>
+      </c>
+      <c r="K33">
+        <v>1.224</v>
+      </c>
+      <c r="L33">
+        <v>0.87</v>
+      </c>
+      <c r="M33" t="s">
+        <v>335</v>
+      </c>
+      <c r="N33" t="s">
+        <v>370</v>
+      </c>
+      <c r="O33">
+        <v>0.8</v>
+      </c>
+      <c r="P33">
+        <v>3</v>
+      </c>
+      <c r="Q33">
+        <v>0.01</v>
+      </c>
+      <c r="R33" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>318</v>
+      </c>
+      <c r="D34">
+        <v>250</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>6.2</v>
+      </c>
+      <c r="K34">
+        <v>1.224</v>
+      </c>
+      <c r="L34">
+        <v>0.87</v>
+      </c>
+      <c r="M34" t="s">
+        <v>335</v>
+      </c>
+      <c r="N34" t="s">
+        <v>371</v>
+      </c>
+      <c r="O34">
+        <v>0.8</v>
+      </c>
+      <c r="P34">
+        <v>3</v>
+      </c>
+      <c r="Q34">
+        <v>0.01</v>
+      </c>
+      <c r="R34" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C35" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="27">
-        <v>310</v>
-      </c>
-      <c r="D3" s="27">
+      <c r="D35">
+        <v>300</v>
+      </c>
+      <c r="E35">
         <v>5</v>
       </c>
-      <c r="E3" s="27">
+      <c r="F35">
         <v>1</v>
       </c>
-      <c r="F3" s="27">
+      <c r="G35">
         <v>1</v>
       </c>
-      <c r="G3" s="27">
+      <c r="H35">
         <v>1</v>
       </c>
-      <c r="H3" s="27">
-        <v>0</v>
-      </c>
-      <c r="I3" s="27">
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
         <v>6.2</v>
       </c>
-      <c r="J3" s="27">
+      <c r="K35">
         <v>1.44</v>
       </c>
-      <c r="K3" s="27">
+      <c r="L35">
         <v>0.87</v>
       </c>
-      <c r="L3" s="27" t="s">
-        <v>328</v>
-      </c>
-      <c r="M3" s="27" t="s">
-        <v>336</v>
-      </c>
-      <c r="N3" s="27">
+      <c r="M35" t="s">
+        <v>334</v>
+      </c>
+      <c r="N35" t="s">
+        <v>337</v>
+      </c>
+      <c r="O35">
         <v>0.8</v>
       </c>
-      <c r="O3" s="27">
+      <c r="P35">
         <v>3</v>
       </c>
-      <c r="P3" s="27">
-        <v>1E-3</v>
-      </c>
-      <c r="Q3" s="27" t="b">
-        <v>0</v>
+      <c r="Q35">
+        <v>0.01</v>
+      </c>
+      <c r="R35" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -2513,7 +4777,7 @@
   <dimension ref="A1:BF219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40758,10 +43022,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:BF219">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="1" stopIfTrue="1">
       <formula>ROW(A2)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="2" stopIfTrue="1">
       <formula>COLUMN(A2)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41089,17 +43353,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43da31f6e8d8dfaec40561525ce78865">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b58fc7e6f492e58d10793199fba37542" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="293b87d96ae3165967deaddc9dd3a283">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23a07973a4b986d214a26a52ed717842" ns3:_="" ns4:_="">
     <xsd:import namespace="871f9270-bc3b-4105-9923-e7982e1cb312"/>
     <xsd:import namespace="000447b7-86fa-4362-939e-855579e16124"/>
     <xsd:element name="properties">
@@ -41118,6 +43373,8 @@
                 <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -41163,6 +43420,18 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -41300,16 +43569,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
     <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -41318,15 +43596,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE8DA1A1-DD54-4881-BC06-911C3C5870BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F180E9D4-9FDD-4A56-9DA9-89F9C4750A22}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -41342,4 +43612,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
prep for batch execution development
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1896157_ed_ac_uk/Documents/Rafael/Models/MaxProfitFeeding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1896157\OneDrive - University of Edinburgh\Rafael\Models\MaxProfitFeeding\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -320,7 +320,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="376">
   <si>
     <t>IFN</t>
   </si>
@@ -1443,6 +1443,12 @@
   <si>
     <t>Add Jair on gitHUb</t>
   </si>
+  <si>
+    <t>.\config.py</t>
+  </si>
+  <si>
+    <t>Add new sheet and column names</t>
+  </si>
 </sst>
 </file>
 
@@ -1584,25 +1590,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="70">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0;0.0;0;@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1899,6 +1886,22 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -1956,6 +1959,9 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1970,13 +1976,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:D10" totalsRowShown="0">
+  <autoFilter ref="A1:D10"/>
   <sortState ref="A2:D9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="TODO" dataDxfId="0"/>
+    <tableColumn id="1" name="TODO" dataDxfId="69"/>
     <tableColumn id="4" name="Meliante"/>
     <tableColumn id="2" name="Script"/>
     <tableColumn id="3" name="Description"/>
@@ -1986,18 +1992,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F37" totalsRowShown="0" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:F37" totalsRowShown="0" dataDxfId="68">
   <autoFilter ref="A1:F37"/>
   <sortState ref="B2:F30">
     <sortCondition ref="B1:B30"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="6" name="Feed Scenario" dataDxfId="68"/>
-    <tableColumn id="1" name="ID" dataDxfId="67"/>
-    <tableColumn id="2" name="Min %DM" dataDxfId="66"/>
-    <tableColumn id="3" name="Max %DM" dataDxfId="65"/>
-    <tableColumn id="4" name="Cost [US$/kg AF]" dataDxfId="64"/>
-    <tableColumn id="5" name="Name" dataDxfId="63">
+    <tableColumn id="6" name="Feed Scenario" dataDxfId="67"/>
+    <tableColumn id="1" name="ID" dataDxfId="66"/>
+    <tableColumn id="2" name="Min %DM" dataDxfId="65"/>
+    <tableColumn id="3" name="Max %DM" dataDxfId="64"/>
+    <tableColumn id="4" name="Cost [US$/kg AF]" dataDxfId="63"/>
+    <tableColumn id="5" name="Name" dataDxfId="62">
       <calculatedColumnFormula>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2048,70 +2054,70 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FeedLib" displayName="FeedLib" ref="A1:BF219" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A1:BF219"/>
   <sortState ref="A2:BF219">
     <sortCondition ref="A4:A5"/>
   </sortState>
   <tableColumns count="58">
-    <tableColumn id="1" name="ID" dataDxfId="60"/>
-    <tableColumn id="2" name="Feed" dataDxfId="59"/>
-    <tableColumn id="4" name="IFN" dataDxfId="58"/>
-    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="57"/>
-    <tableColumn id="7" name="Forage, %DM" dataDxfId="56"/>
-    <tableColumn id="8" name="DM, %AF" dataDxfId="55"/>
-    <tableColumn id="16" name="CP, %DM" dataDxfId="54"/>
-    <tableColumn id="31" name="SP, %CP" dataDxfId="53"/>
-    <tableColumn id="29" name="ADICP, %CP" dataDxfId="52"/>
-    <tableColumn id="24" name="Sugars, %DM" dataDxfId="51"/>
-    <tableColumn id="25" name="OA, %DM" dataDxfId="50"/>
-    <tableColumn id="23" name="Fat, %DM" dataDxfId="49"/>
-    <tableColumn id="9" name="Ash, %DM" dataDxfId="48"/>
-    <tableColumn id="10" name="Starch, %DM" dataDxfId="47"/>
-    <tableColumn id="12" name="NDF, %DM" dataDxfId="46"/>
-    <tableColumn id="13" name="Lignin, %DM" dataDxfId="45"/>
-    <tableColumn id="14" name="TDN, %DM" dataDxfId="44"/>
-    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="43"/>
-    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="42"/>
-    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="41"/>
-    <tableColumn id="21" name="RUP, %CP" dataDxfId="40"/>
-    <tableColumn id="22" name="kd PB, %/h" dataDxfId="39"/>
-    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="38"/>
-    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="37"/>
-    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="36"/>
-    <tableColumn id="28" name="PBID, %" dataDxfId="35"/>
-    <tableColumn id="6" name="CB1ID, %" dataDxfId="34"/>
-    <tableColumn id="3" name="CB2ID, %" dataDxfId="33"/>
-    <tableColumn id="20" name="pef, %NDF" dataDxfId="32"/>
-    <tableColumn id="11" name="ARG, %DM" dataDxfId="31"/>
-    <tableColumn id="32" name="HIS, %DM" dataDxfId="30"/>
-    <tableColumn id="33" name="ILE, %DM" dataDxfId="29"/>
-    <tableColumn id="34" name="LEU, %DM" dataDxfId="28"/>
-    <tableColumn id="35" name="LYS, %DM" dataDxfId="27"/>
-    <tableColumn id="36" name="MET, %DM" dataDxfId="26"/>
-    <tableColumn id="37" name="CYS, %DM" dataDxfId="25"/>
-    <tableColumn id="38" name="PHE, %DM" dataDxfId="24"/>
-    <tableColumn id="39" name="TYR, %DM" dataDxfId="23"/>
-    <tableColumn id="40" name="THR, %DM" dataDxfId="22"/>
-    <tableColumn id="41" name="TRP, %DM" dataDxfId="21"/>
-    <tableColumn id="42" name="VAL, %DM" dataDxfId="20"/>
-    <tableColumn id="43" name="Ca, % DM" dataDxfId="19"/>
-    <tableColumn id="44" name="P, % DM" dataDxfId="18"/>
-    <tableColumn id="45" name="Mg, % DM" dataDxfId="17"/>
-    <tableColumn id="46" name="Cl, % DM" dataDxfId="16"/>
-    <tableColumn id="47" name="K, % DM" dataDxfId="15"/>
-    <tableColumn id="48" name="Na, % DM" dataDxfId="14"/>
-    <tableColumn id="49" name="S, % DM" dataDxfId="13"/>
-    <tableColumn id="50" name="Co, mg/kg" dataDxfId="12"/>
-    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="11"/>
-    <tableColumn id="52" name="I, mg/kg" dataDxfId="10"/>
-    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="9"/>
-    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="8"/>
-    <tableColumn id="55" name="Se, mg/kg" dataDxfId="7"/>
-    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="6"/>
-    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="5"/>
-    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="4"/>
-    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="3"/>
+    <tableColumn id="1" name="ID" dataDxfId="57"/>
+    <tableColumn id="2" name="Feed" dataDxfId="56"/>
+    <tableColumn id="4" name="IFN" dataDxfId="55"/>
+    <tableColumn id="5" name="Cost, $/Tonne AF" dataDxfId="54"/>
+    <tableColumn id="7" name="Forage, %DM" dataDxfId="53"/>
+    <tableColumn id="8" name="DM, %AF" dataDxfId="52"/>
+    <tableColumn id="16" name="CP, %DM" dataDxfId="51"/>
+    <tableColumn id="31" name="SP, %CP" dataDxfId="50"/>
+    <tableColumn id="29" name="ADICP, %CP" dataDxfId="49"/>
+    <tableColumn id="24" name="Sugars, %DM" dataDxfId="48"/>
+    <tableColumn id="25" name="OA, %DM" dataDxfId="47"/>
+    <tableColumn id="23" name="Fat, %DM" dataDxfId="46"/>
+    <tableColumn id="9" name="Ash, %DM" dataDxfId="45"/>
+    <tableColumn id="10" name="Starch, %DM" dataDxfId="44"/>
+    <tableColumn id="12" name="NDF, %DM" dataDxfId="43"/>
+    <tableColumn id="13" name="Lignin, %DM" dataDxfId="42"/>
+    <tableColumn id="14" name="TDN, %DM" dataDxfId="41"/>
+    <tableColumn id="15" name="ME, Mcal/kg" dataDxfId="40"/>
+    <tableColumn id="18" name="NEma, Mcal/kg" dataDxfId="39"/>
+    <tableColumn id="19" name="NEga, Mcal/kg" dataDxfId="38"/>
+    <tableColumn id="21" name="RUP, %CP" dataDxfId="37"/>
+    <tableColumn id="22" name="kd PB, %/h" dataDxfId="36"/>
+    <tableColumn id="26" name="kd CB1, %/h" dataDxfId="35"/>
+    <tableColumn id="27" name="kd CB2, %/h" dataDxfId="34"/>
+    <tableColumn id="17" name="kd CB3, %/h" dataDxfId="33"/>
+    <tableColumn id="28" name="PBID, %" dataDxfId="32"/>
+    <tableColumn id="6" name="CB1ID, %" dataDxfId="31"/>
+    <tableColumn id="3" name="CB2ID, %" dataDxfId="30"/>
+    <tableColumn id="20" name="pef, %NDF" dataDxfId="29"/>
+    <tableColumn id="11" name="ARG, %DM" dataDxfId="28"/>
+    <tableColumn id="32" name="HIS, %DM" dataDxfId="27"/>
+    <tableColumn id="33" name="ILE, %DM" dataDxfId="26"/>
+    <tableColumn id="34" name="LEU, %DM" dataDxfId="25"/>
+    <tableColumn id="35" name="LYS, %DM" dataDxfId="24"/>
+    <tableColumn id="36" name="MET, %DM" dataDxfId="23"/>
+    <tableColumn id="37" name="CYS, %DM" dataDxfId="22"/>
+    <tableColumn id="38" name="PHE, %DM" dataDxfId="21"/>
+    <tableColumn id="39" name="TYR, %DM" dataDxfId="20"/>
+    <tableColumn id="40" name="THR, %DM" dataDxfId="19"/>
+    <tableColumn id="41" name="TRP, %DM" dataDxfId="18"/>
+    <tableColumn id="42" name="VAL, %DM" dataDxfId="17"/>
+    <tableColumn id="43" name="Ca, % DM" dataDxfId="16"/>
+    <tableColumn id="44" name="P, % DM" dataDxfId="15"/>
+    <tableColumn id="45" name="Mg, % DM" dataDxfId="14"/>
+    <tableColumn id="46" name="Cl, % DM" dataDxfId="13"/>
+    <tableColumn id="47" name="K, % DM" dataDxfId="12"/>
+    <tableColumn id="48" name="Na, % DM" dataDxfId="11"/>
+    <tableColumn id="49" name="S, % DM" dataDxfId="10"/>
+    <tableColumn id="50" name="Co, mg/kg" dataDxfId="9"/>
+    <tableColumn id="51" name="Cu, mg/kg" dataDxfId="8"/>
+    <tableColumn id="52" name="I, mg/kg" dataDxfId="7"/>
+    <tableColumn id="53" name="Fe, mg/kg" dataDxfId="6"/>
+    <tableColumn id="54" name="Mn, mg/kg" dataDxfId="5"/>
+    <tableColumn id="55" name="Se, mg/kg" dataDxfId="4"/>
+    <tableColumn id="56" name="Zn, mg/kg" dataDxfId="3"/>
+    <tableColumn id="57" name="Vit A, IU/g" dataDxfId="2"/>
+    <tableColumn id="58" name="Vit D, IU/g" dataDxfId="1"/>
+    <tableColumn id="30" name="Vit E, IU/kg" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2383,10 +2389,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2517,6 +2523,20 @@
       </c>
       <c r="D9" t="s">
         <v>368</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>370</v>
+      </c>
+      <c r="C10" t="s">
+        <v>374</v>
+      </c>
+      <c r="D10" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -41999,10 +42019,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:BF219">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="1" stopIfTrue="1">
       <formula>ROW(A2)=$E$1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="2" stopIfTrue="1">
       <formula>COLUMN(A2)=$F$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42324,12 +42344,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C4402FDC8975A4FB65AB474AF423692" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="293b87d96ae3165967deaddc9dd3a283">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="871f9270-bc3b-4105-9923-e7982e1cb312" xmlns:ns4="000447b7-86fa-4362-939e-855579e16124" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="23a07973a4b986d214a26a52ed717842" ns3:_="" ns4:_="">
     <xsd:import namespace="871f9270-bc3b-4105-9923-e7982e1cb312"/>
@@ -42546,6 +42560,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -42556,23 +42576,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F180E9D4-9FDD-4A56-9DA9-89F9C4750A22}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42591,6 +42594,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9544B578-CE8A-4753-8E47-B2C52E32EEC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="000447b7-86fa-4362-939e-855579e16124"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="871f9270-bc3b-4105-9923-e7982e1cb312"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C60666F-AED0-4727-A902-9CA0ACF4D344}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Batch implementation input tested
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TODOS" sheetId="1" r:id="rId1"/>
@@ -114,32 +114,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">MARQUES Gabriel:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>0.11</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="E19" authorId="0" shapeId="0">
       <text>
         <r>
@@ -163,33 +137,6 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">0.14
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">MARQUES Gabriel:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">0.1
 </t>
         </r>
       </text>
@@ -2620,6 +2567,486 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 20"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 18"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 16"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 14"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 12"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 10"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 8"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2684,6 +3111,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7620000" cy="7620000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3290,8 +3765,8 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3590,8 +4065,8 @@
       <c r="D14" s="4">
         <v>100</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>25</v>
+      <c r="E14" s="5">
+        <v>0.2</v>
       </c>
       <c r="F14" s="4" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -3674,8 +4149,8 @@
       <c r="D18" s="4">
         <v>100</v>
       </c>
-      <c r="E18" s="5">
-        <v>0.14000000000000001</v>
+      <c r="E18" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="F18" s="4" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -3696,7 +4171,7 @@
         <v>100</v>
       </c>
       <c r="E19" s="5">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="F19" s="4" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -3716,8 +4191,8 @@
       <c r="D20" s="4">
         <v>100</v>
       </c>
-      <c r="E20" s="5">
-        <v>0.14000000000000001</v>
+      <c r="E20" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="F20" s="4" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -3737,8 +4212,8 @@
       <c r="D21" s="4">
         <v>100</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>26</v>
+      <c r="E21" s="5">
+        <v>0.3</v>
       </c>
       <c r="F21" s="4" t="str">
         <f>VLOOKUP(Tabela2[[#This Row],[ID]],FeedLib[],2,0)</f>
@@ -4099,7 +4574,7 @@
   </sheetPr>
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>

</xml_diff>